<commit_message>
Added full Authorization functionality and check on FYP submission form @ConnorSF 27.05.2020
</commit_message>
<xml_diff>
--- a/Test Data Imports/imports-special.xlsx
+++ b/Test Data Imports/imports-special.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\conno\source\repos\GAPT\Test Data Imports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B964F6-A5DB-4B59-9F55-8A518B8AD73D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDDCCFB-77BA-410B-997B-89B7CF89F92E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6930" yWindow="810" windowWidth="13260" windowHeight="11670" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4950" yWindow="1335" windowWidth="13260" windowHeight="11670" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -615,9 +615,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -912,7 +913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2:E23"/>
     </sheetView>
   </sheetViews>
@@ -1318,14 +1319,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C43" sqref="C2:C43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="2"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="2" t="s">
         <v>85</v>
       </c>
       <c r="B1" t="s">
@@ -1339,7 +1343,7 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
+      <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
@@ -1353,7 +1357,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1">
+      <c r="A3" s="2">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -1367,7 +1371,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="1">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -1381,7 +1385,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="1">
+      <c r="A5" s="2">
         <v>1</v>
       </c>
       <c r="B5" t="s">
@@ -1395,7 +1399,7 @@
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1">
+      <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" t="s">
@@ -1409,7 +1413,7 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
+      <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" t="s">
@@ -1423,7 +1427,7 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
+      <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" t="s">
@@ -1437,7 +1441,7 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="1">
+      <c r="A9" s="2">
         <v>2</v>
       </c>
       <c r="B9" t="s">
@@ -1451,7 +1455,7 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
+      <c r="A10" s="2">
         <v>2</v>
       </c>
       <c r="B10" t="s">
@@ -1465,7 +1469,7 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
+      <c r="A11" s="2">
         <v>2</v>
       </c>
       <c r="B11" t="s">
@@ -1479,7 +1483,7 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
+      <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" t="s">
@@ -1493,7 +1497,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="1">
+      <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" t="s">
@@ -1507,7 +1511,7 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
+      <c r="A14" s="2">
         <v>2</v>
       </c>
       <c r="B14" t="s">
@@ -1521,7 +1525,7 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="1">
+      <c r="A15" s="2">
         <v>2</v>
       </c>
       <c r="B15" t="s">
@@ -1535,7 +1539,7 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
+      <c r="A16" s="2">
         <v>3</v>
       </c>
       <c r="B16" t="s">
@@ -1549,7 +1553,7 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="1">
+      <c r="A17" s="2">
         <v>3</v>
       </c>
       <c r="B17" t="s">
@@ -1563,7 +1567,7 @@
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="1">
+      <c r="A18" s="2">
         <v>3</v>
       </c>
       <c r="B18" t="s">
@@ -1577,7 +1581,7 @@
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="1">
+      <c r="A19" s="2">
         <v>3</v>
       </c>
       <c r="B19" t="s">
@@ -1591,7 +1595,7 @@
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="1">
+      <c r="A20" s="2">
         <v>3</v>
       </c>
       <c r="B20" t="s">
@@ -1605,7 +1609,7 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
+      <c r="A21" s="2">
         <v>3</v>
       </c>
       <c r="B21" t="s">
@@ -1619,7 +1623,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
+      <c r="A22" s="2">
         <v>3</v>
       </c>
       <c r="B22" t="s">
@@ -1633,7 +1637,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
+      <c r="A23" s="2">
         <v>4</v>
       </c>
       <c r="B23" t="s">
@@ -1647,7 +1651,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
+      <c r="A24" s="2">
         <v>4</v>
       </c>
       <c r="B24" t="s">
@@ -1661,7 +1665,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
+      <c r="A25" s="2">
         <v>4</v>
       </c>
       <c r="B25" t="s">
@@ -1675,7 +1679,7 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
+      <c r="A26" s="2">
         <v>4</v>
       </c>
       <c r="B26" t="s">
@@ -1689,7 +1693,7 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
+      <c r="A27" s="2">
         <v>4</v>
       </c>
       <c r="B27" t="s">
@@ -1703,7 +1707,7 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
+      <c r="A28" s="2">
         <v>4</v>
       </c>
       <c r="B28" t="s">
@@ -1717,7 +1721,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="1">
+      <c r="A29" s="2">
         <v>4</v>
       </c>
       <c r="B29" t="s">
@@ -1731,7 +1735,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="1">
+      <c r="A30" s="2">
         <v>5</v>
       </c>
       <c r="B30" t="s">
@@ -1745,7 +1749,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="1">
+      <c r="A31" s="2">
         <v>5</v>
       </c>
       <c r="B31" t="s">
@@ -1759,7 +1763,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="1">
+      <c r="A32" s="2">
         <v>5</v>
       </c>
       <c r="B32" t="s">
@@ -1773,7 +1777,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="1">
+      <c r="A33" s="2">
         <v>5</v>
       </c>
       <c r="B33" t="s">
@@ -1787,7 +1791,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="1">
+      <c r="A34" s="2">
         <v>5</v>
       </c>
       <c r="B34" t="s">
@@ -1801,7 +1805,7 @@
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="1">
+      <c r="A35" s="2">
         <v>5</v>
       </c>
       <c r="B35" t="s">
@@ -1815,7 +1819,7 @@
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="1">
+      <c r="A36" s="2">
         <v>5</v>
       </c>
       <c r="B36" t="s">
@@ -1829,7 +1833,7 @@
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1">
+      <c r="A37" s="2">
         <v>6</v>
       </c>
       <c r="B37" t="s">
@@ -1843,7 +1847,7 @@
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1">
+      <c r="A38" s="2">
         <v>6</v>
       </c>
       <c r="B38" t="s">
@@ -1857,7 +1861,7 @@
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1">
+      <c r="A39" s="2">
         <v>6</v>
       </c>
       <c r="B39" t="s">
@@ -1871,7 +1875,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="1">
+      <c r="A40" s="2">
         <v>6</v>
       </c>
       <c r="B40" t="s">
@@ -1885,7 +1889,7 @@
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="1">
+      <c r="A41" s="2">
         <v>6</v>
       </c>
       <c r="B41" t="s">
@@ -1899,7 +1903,7 @@
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="1">
+      <c r="A42" s="2">
         <v>6</v>
       </c>
       <c r="B42" t="s">
@@ -1913,7 +1917,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="1">
+      <c r="A43" s="2">
         <v>6</v>
       </c>
       <c r="B43" t="s">
@@ -1928,6 +1932,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>